<commit_message>
added a function for approving ipcr and optimized opcr generation
</commit_message>
<xml_diff>
--- a/excels/OPCRTest.xlsx
+++ b/excels/OPCRTest.xlsx
@@ -815,13 +815,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="609600" cy="466725"/>
+    <xdr:ext cx="609600" cy="571500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -842,14 +842,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="647700" cy="504825"/>
+    <xdr:ext cx="647700" cy="619125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1172,7 +1172,7 @@
       <c r="R4" s="2"/>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
+    <row r="5" ht="28.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -2789,37 +2789,37 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A5:S5"/>
-    <mergeCell ref="A6:S6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
     <mergeCell ref="A4:S4"/>
+    <mergeCell ref="A5:S5"/>
+    <mergeCell ref="A6:S6"/>
     <mergeCell ref="A7:S7"/>
-    <mergeCell ref="N22:Q23"/>
-    <mergeCell ref="R22:S24"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A26:S26"/>
+    <mergeCell ref="N8:S8"/>
+    <mergeCell ref="N9:S9"/>
+    <mergeCell ref="N10:S10"/>
+    <mergeCell ref="N11:S11"/>
+    <mergeCell ref="A12:G12"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A22:C24"/>
-    <mergeCell ref="D22:G24"/>
-    <mergeCell ref="H22:H24"/>
     <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A12:G12"/>
     <mergeCell ref="O16:P16"/>
     <mergeCell ref="R16:S16"/>
     <mergeCell ref="R17:S17"/>
     <mergeCell ref="R18:S18"/>
     <mergeCell ref="R19:S19"/>
     <mergeCell ref="R20:S20"/>
-    <mergeCell ref="N8:S8"/>
-    <mergeCell ref="N9:S9"/>
-    <mergeCell ref="N10:S10"/>
-    <mergeCell ref="N11:S11"/>
+    <mergeCell ref="R22:S24"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="A22:C24"/>
+    <mergeCell ref="D22:G24"/>
+    <mergeCell ref="H22:H24"/>
     <mergeCell ref="I22:I24"/>
     <mergeCell ref="J22:M24"/>
+    <mergeCell ref="N22:Q23"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:S26"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.0" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.0"/>

</xml_diff>